<commit_message>
update to Internal Fitbit Inventory
</commit_message>
<xml_diff>
--- a/fitbitIntegration/InternalFitbitInventory.xlsx
+++ b/fitbitIntegration/InternalFitbitInventory.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>FBHRO1</t>
   </si>
@@ -79,12 +79,15 @@
   </si>
   <si>
     <t>"Center's Watch"</t>
+  </si>
+  <si>
+    <t>Aug 29th, 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,24 +398,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -438,7 +441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -461,7 +464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -482,6 +485,52 @@
       </c>
       <c r="G3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to Fitbit Inventory
</commit_message>
<xml_diff>
--- a/fitbitIntegration/InternalFitbitInventory.xlsx
+++ b/fitbitIntegration/InternalFitbitInventory.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>FBHRO1</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Aug 29th, 2017</t>
+  </si>
+  <si>
+    <t>Iqra</t>
+  </si>
+  <si>
+    <t>Dec 14th, 2017</t>
+  </si>
+  <si>
+    <t>Tech Ops</t>
+  </si>
+  <si>
+    <t>Alana</t>
+  </si>
+  <si>
+    <t>Jan 29th, 2018</t>
+  </si>
+  <si>
+    <t>Jan 12th, 2018</t>
   </si>
 </sst>
 </file>
@@ -399,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +551,81 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>